<commit_message>
datos limpios excel metrobus
</commit_message>
<xml_diff>
--- a/database/Fuentes/lineas-y-estaciones-del-metrobus0.xlsx
+++ b/database/Fuentes/lineas-y-estaciones-del-metrobus0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guagnelli/.bitnami/stackman/machines/xampp/volumes/root/htdocs/tejiendo_ciudad/database/Fuentes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\tejiendo_ciudad\database\Fuentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D493107C-0EDC-C344-B56E-C8B4A9661A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C463EA-E43C-42EB-A441-23579D20360B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lineas-y-estaciones-del-metrobu" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="263">
   <si>
     <t>latitud</t>
   </si>
@@ -79,30 +79,15 @@
     <t>MB04-N (San Lazaro - Buenavista)</t>
   </si>
   <si>
-    <t>E√∫zkaro</t>
-  </si>
-  <si>
-    <t>San Sim√≥n</t>
-  </si>
-  <si>
-    <t>Manuel Gonz√°lez</t>
-  </si>
-  <si>
     <t>Buenavista</t>
   </si>
   <si>
-    <t>Revoluci√≥n</t>
-  </si>
-  <si>
     <t>Durango</t>
   </si>
   <si>
     <t>Campeche</t>
   </si>
   <si>
-    <t>Polif√≥rum</t>
-  </si>
-  <si>
     <t>Francia</t>
   </si>
   <si>
@@ -121,24 +106,12 @@
     <t>Patriotismo</t>
   </si>
   <si>
-    <t>Nuevo Le√≥n</t>
-  </si>
-  <si>
-    <t>√Ålamos</t>
-  </si>
-  <si>
     <t>Tlacotal</t>
   </si>
   <si>
     <t>Goma</t>
   </si>
   <si>
-    <t>R√≠o Mayo</t>
-  </si>
-  <si>
-    <t>Rojo G√≥mez</t>
-  </si>
-  <si>
     <t>Del Moral</t>
   </si>
   <si>
@@ -163,24 +136,9 @@
     <t>Hidalgo</t>
   </si>
   <si>
-    <t>Jard√≠n Pushkin</t>
-  </si>
-  <si>
-    <t>Etiop√≠a</t>
-  </si>
-  <si>
-    <t>Glorieta de Col√≥n</t>
-  </si>
-  <si>
     <t>Expo Reforma</t>
   </si>
   <si>
-    <t>Ju√°rez</t>
-  </si>
-  <si>
-    <t>Isabel la Cat√≥lica</t>
-  </si>
-  <si>
     <t>Museo de la Ciudad</t>
   </si>
   <si>
@@ -217,36 +175,15 @@
     <t>Canal del Norte</t>
   </si>
   <si>
-    <t>R√≠o Santa Coleta</t>
-  </si>
-  <si>
     <t>Victoria</t>
   </si>
   <si>
-    <t>R√≠o de Los Remedios</t>
-  </si>
-  <si>
-    <t>Francisco Moraz√°n</t>
-  </si>
-  <si>
-    <t>Volc√°n de Fuego</t>
-  </si>
-  <si>
-    <t>Ampliaci√≥n Providencia</t>
-  </si>
-  <si>
     <t>Deportivo Los Galeana</t>
   </si>
   <si>
-    <t>Casas Alem√°n</t>
-  </si>
-  <si>
     <t>Gran Canal</t>
   </si>
   <si>
-    <t>Instituto Polit√©cnico Nacional</t>
-  </si>
-  <si>
     <t>San Bartolo</t>
   </si>
   <si>
@@ -262,21 +199,12 @@
     <t>De Los Misterios</t>
   </si>
   <si>
-    <t>Delegaci√≥n Gustavo A. Madero</t>
-  </si>
-  <si>
     <t>Hospital Infantil La Villa</t>
   </si>
   <si>
-    <t>Av. Talism√°n</t>
-  </si>
-  <si>
     <t>Necaxa</t>
   </si>
   <si>
-    <t>Exc√©lsior</t>
-  </si>
-  <si>
     <t>Clave</t>
   </si>
   <si>
@@ -292,18 +220,12 @@
     <t>Tres Culturas</t>
   </si>
   <si>
-    <t>Glorieta Cuitl√°huac</t>
-  </si>
-  <si>
     <t>Reforma</t>
   </si>
   <si>
     <t>Hamburgo</t>
   </si>
   <si>
-    <t>El √Ångel</t>
-  </si>
-  <si>
     <t>La Diana</t>
   </si>
   <si>
@@ -370,9 +292,6 @@
     <t>El Chopo</t>
   </si>
   <si>
-    <t>Plaza de la Rep√∫blica</t>
-  </si>
-  <si>
     <t>Insurgentes</t>
   </si>
   <si>
@@ -382,21 +301,12 @@
     <t>Colonia del Valle</t>
   </si>
   <si>
-    <t>F√©lix Cuevas</t>
-  </si>
-  <si>
-    <t>Jos√© Mar√≠a Velasco</t>
-  </si>
-  <si>
     <t>Olivo</t>
   </si>
   <si>
     <t>La Piedad</t>
   </si>
   <si>
-    <t>Villa Ol√≠mpica</t>
-  </si>
-  <si>
     <t>Corregidora</t>
   </si>
   <si>
@@ -409,9 +319,6 @@
     <t>Parque Lira</t>
   </si>
   <si>
-    <t>Escand√≥n</t>
-  </si>
-  <si>
     <t>Xola</t>
   </si>
   <si>
@@ -430,111 +337,57 @@
     <t>El Rodeo</t>
   </si>
   <si>
-    <t>R√≠o Tecolutla</t>
-  </si>
-  <si>
-    <t>R√≠o Fr√≠o</t>
-  </si>
-  <si>
     <t>Leyes de Reforma</t>
   </si>
   <si>
     <t>CCH Oriente</t>
   </si>
   <si>
-    <t>General Antonio de Le√≥n</t>
-  </si>
-  <si>
-    <t>Nicol√°s Bravo</t>
-  </si>
-  <si>
     <t>Tenayuca</t>
   </si>
   <si>
-    <t>San Jos√© de la Escalera</t>
-  </si>
-  <si>
     <t>Poniente 128</t>
   </si>
   <si>
     <t>Magdalena de las Salinas</t>
   </si>
   <si>
-    <t>Cuitl√°huac</t>
-  </si>
-  <si>
-    <t>H√©roe de Nacozari</t>
-  </si>
-  <si>
-    <t>Tolnahu√°c</t>
-  </si>
-  <si>
     <t>Mina</t>
   </si>
   <si>
     <t>Balderas</t>
   </si>
   <si>
-    <t>Cuauht√©moc</t>
-  </si>
-  <si>
-    <t>Centro M√©dico</t>
-  </si>
-  <si>
     <t>Obrero Mundial</t>
   </si>
   <si>
     <t>El Salvador</t>
   </si>
   <si>
-    <t>Pino Su√°rez</t>
-  </si>
-  <si>
-    <t>Circunvalaci√≥n</t>
-  </si>
-  <si>
     <t>Hospital Balbuena</t>
   </si>
   <si>
     <t>Teatro del Pueblo</t>
   </si>
   <si>
-    <t>Rep√∫blica de Argentina</t>
-  </si>
-  <si>
-    <t>Rep√∫blica de Chile</t>
-  </si>
-  <si>
     <t>Bellas Artes</t>
   </si>
   <si>
-    <t>R√≠o Consulado</t>
-  </si>
-  <si>
     <t>Oriente 101</t>
   </si>
   <si>
-    <t>San Juan de Arag√≥n</t>
-  </si>
-  <si>
     <t>El Coyol</t>
   </si>
   <si>
     <t>5 de Mayo</t>
   </si>
   <si>
-    <t>Villa de Arag√≥n</t>
-  </si>
-  <si>
     <t>La Pradera</t>
   </si>
   <si>
     <t>416 Poniente</t>
   </si>
   <si>
-    <t>Mart√≠n Carrera</t>
-  </si>
-  <si>
     <t>Riobamba</t>
   </si>
   <si>
@@ -550,51 +403,30 @@
     <t>Garibaldi</t>
   </si>
   <si>
-    <t>Par√≠s</t>
-  </si>
-  <si>
-    <t>Antropolog√≠a</t>
-  </si>
-  <si>
     <t>Deportivo 18 de Marzo</t>
   </si>
   <si>
     <t>Potrero</t>
   </si>
   <si>
-    <t>√Ålvaro Obreg√≥n</t>
-  </si>
-  <si>
     <t>Chilpancingo</t>
   </si>
   <si>
-    <t>N√°poles</t>
-  </si>
-  <si>
     <t>Ciudad de los Deportes</t>
   </si>
   <si>
     <t>Parque Hundido</t>
   </si>
   <si>
-    <t>R√≠o Churubusco</t>
-  </si>
-  <si>
     <t>Teatro de los Insurgentes</t>
   </si>
   <si>
-    <t>Doctor G√°lvez</t>
-  </si>
-  <si>
     <t>Ciudad Universitaria</t>
   </si>
   <si>
     <t>Perisur</t>
   </si>
   <si>
-    <t>Santa √örsula</t>
-  </si>
-  <si>
     <t>El Caminero</t>
   </si>
   <si>
@@ -613,24 +445,12 @@
     <t>Amores</t>
   </si>
   <si>
-    <t>Doctor V√©rtiz</t>
-  </si>
-  <si>
     <t>Centro SCOP</t>
   </si>
   <si>
-    <t>Las Am√©ricas</t>
-  </si>
-  <si>
-    <t>Andr√©s Molina</t>
-  </si>
-  <si>
     <t>Canela</t>
   </si>
   <si>
-    <t>Constituci√≥n de Apatzing√°n</t>
-  </si>
-  <si>
     <t>Tepalcates</t>
   </si>
   <si>
@@ -643,9 +463,6 @@
     <t>Tres Anegas</t>
   </si>
   <si>
-    <t>J√∫piter</t>
-  </si>
-  <si>
     <t>La Patera</t>
   </si>
   <si>
@@ -655,18 +472,9 @@
     <t>Tlatelolco</t>
   </si>
   <si>
-    <t>Ricardo Flores Mag√≥n</t>
-  </si>
-  <si>
     <t>Hospital General</t>
   </si>
   <si>
-    <t>Doctor M√°rquez</t>
-  </si>
-  <si>
-    <t>Delegaci√≥n Cuauht√©moc</t>
-  </si>
-  <si>
     <t>Puente de Alvarado</t>
   </si>
   <si>
@@ -682,9 +490,6 @@
     <t>Merced</t>
   </si>
   <si>
-    <t>Archivo General de la Naci√≥n</t>
-  </si>
-  <si>
     <t>Teatro Blanquita</t>
   </si>
   <si>
@@ -700,9 +505,6 @@
     <t>Deportivo Eduardo Molina</t>
   </si>
   <si>
-    <t>Talism√°n</t>
-  </si>
-  <si>
     <t>R√≠o de Guadalupe</t>
   </si>
   <si>
@@ -721,18 +523,12 @@
     <t>Loreto Fabela</t>
   </si>
   <si>
-    <t>Pueblo San Juan de Arag√≥n</t>
-  </si>
-  <si>
     <t>Hospital General La Villa</t>
   </si>
   <si>
     <t>La Villa</t>
   </si>
   <si>
-    <t>Instituto del Petr√≥leo</t>
-  </si>
-  <si>
     <t>Norte 59</t>
   </si>
   <si>
@@ -806,12 +602,219 @@
   </si>
   <si>
     <t>MB03-B (Balderas - Tenayuca)</t>
+  </si>
+  <si>
+    <t>Euzkaro</t>
+  </si>
+  <si>
+    <t>San Simon</t>
+  </si>
+  <si>
+    <t>Manuel Gonzalez</t>
+  </si>
+  <si>
+    <t>Revolucion</t>
+  </si>
+  <si>
+    <t>Polifurum</t>
+  </si>
+  <si>
+    <t>Nuevo Leon</t>
+  </si>
+  <si>
+    <t>Alamos</t>
+  </si>
+  <si>
+    <t>Rio Mayo</t>
+  </si>
+  <si>
+    <t>Rojo Gomez</t>
+  </si>
+  <si>
+    <t>Jardin Pushkin</t>
+  </si>
+  <si>
+    <t>Etiopia</t>
+  </si>
+  <si>
+    <t>Glorieta de Colon</t>
+  </si>
+  <si>
+    <t>Juarez</t>
+  </si>
+  <si>
+    <t>Isabel la Catolica</t>
+  </si>
+  <si>
+    <t>Rio Santa Coleta</t>
+  </si>
+  <si>
+    <t>Rio de Los Remedios</t>
+  </si>
+  <si>
+    <t>Francisco Morazan</t>
+  </si>
+  <si>
+    <t>Volcan de Fuego</t>
+  </si>
+  <si>
+    <t>Ampliacion Providencia</t>
+  </si>
+  <si>
+    <t>Casas Aleman</t>
+  </si>
+  <si>
+    <t>Instituto Politecnico Nacional</t>
+  </si>
+  <si>
+    <t>Delegacion Gustavo A. Madero</t>
+  </si>
+  <si>
+    <t>Av. Talisman</t>
+  </si>
+  <si>
+    <t>Excelsior</t>
+  </si>
+  <si>
+    <t>Glorieta Cuitlahuac</t>
+  </si>
+  <si>
+    <t>El Angel</t>
+  </si>
+  <si>
+    <t>Plaza de la Republica</t>
+  </si>
+  <si>
+    <t>Felix Cuevas</t>
+  </si>
+  <si>
+    <t>Jose Maria Velasco</t>
+  </si>
+  <si>
+    <t>Villa Olimpica</t>
+  </si>
+  <si>
+    <t>Escandon</t>
+  </si>
+  <si>
+    <t>Rio Tecolutla</t>
+  </si>
+  <si>
+    <t>Rio Frio</t>
+  </si>
+  <si>
+    <t>General Antonio de Leon</t>
+  </si>
+  <si>
+    <t>Nicolas Bravo</t>
+  </si>
+  <si>
+    <t>San Jose de la Escalera</t>
+  </si>
+  <si>
+    <t>Cuitlahuac</t>
+  </si>
+  <si>
+    <t>Heroe de Nacozari</t>
+  </si>
+  <si>
+    <t>Tolnahuac</t>
+  </si>
+  <si>
+    <t>Cuauhtemoc</t>
+  </si>
+  <si>
+    <t>Centro Medico</t>
+  </si>
+  <si>
+    <t>Pino Suarez</t>
+  </si>
+  <si>
+    <t>Circunvalacion</t>
+  </si>
+  <si>
+    <t>Republica de Argentina</t>
+  </si>
+  <si>
+    <t>Republica de Chile</t>
+  </si>
+  <si>
+    <t>Rio Consulado</t>
+  </si>
+  <si>
+    <t>San Juan de Aragon</t>
+  </si>
+  <si>
+    <t>Villa de Aragon</t>
+  </si>
+  <si>
+    <t>Martin Carrera</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Antropologia</t>
+  </si>
+  <si>
+    <t>Alvaro Obregon</t>
+  </si>
+  <si>
+    <t>Napoles</t>
+  </si>
+  <si>
+    <t>Rio Churubusco</t>
+  </si>
+  <si>
+    <t>Doctor Galvez</t>
+  </si>
+  <si>
+    <t>Santa Ursula</t>
+  </si>
+  <si>
+    <t>Doctor Vertiz</t>
+  </si>
+  <si>
+    <t>Las Americas</t>
+  </si>
+  <si>
+    <t>Andres Molina</t>
+  </si>
+  <si>
+    <t>Constitucion de Apatzingan</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>Ricardo Flores Magon</t>
+  </si>
+  <si>
+    <t>Doctor Marquez</t>
+  </si>
+  <si>
+    <t>Delegacion Cuauhtemoc</t>
+  </si>
+  <si>
+    <t>San Lazaro</t>
+  </si>
+  <si>
+    <t>Archivo General de la Nacion</t>
+  </si>
+  <si>
+    <t>Instituto del Petroleo</t>
+  </si>
+  <si>
+    <t>Pueblo San Juan de Aragon</t>
+  </si>
+  <si>
+    <t>Talisman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1293,48 +1296,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1350,7 +1353,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1645,14 +1648,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="C250" sqref="C250"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="57.09765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>19.447252429999999</v>
       </c>
@@ -1680,7 +1688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19.392913270000001</v>
       </c>
@@ -1694,7 +1702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19.476998219999999</v>
       </c>
@@ -1708,7 +1716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>19.455501730000002</v>
       </c>
@@ -1722,7 +1730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>19.48567959</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>19.487663049999998</v>
       </c>
@@ -1750,7 +1758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>19.4858364</v>
       </c>
@@ -1764,7 +1772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>19.463091729999999</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>19.430247399999999</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>19.466911280000001</v>
       </c>
@@ -1806,7 +1814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>19.420817060000001</v>
       </c>
@@ -1820,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>19.39211465</v>
       </c>
@@ -1834,7 +1842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>19.496827759999999</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>19.430224450000001</v>
       </c>
@@ -1862,7 +1870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>19.43741872</v>
       </c>
@@ -1876,391 +1884,391 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
         <v>23</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
         <v>26</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
         <v>27</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
         <v>28</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
         <v>29</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
         <v>30</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
         <v>31</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>40</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>47</v>
+        <v>203</v>
       </c>
       <c r="D45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="D46">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>49</v>
+        <v>205</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D48">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>51</v>
+        <v>206</v>
       </c>
       <c r="D49">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>52</v>
+        <v>207</v>
       </c>
       <c r="D50">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D51">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D52">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D53">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D54">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D55">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D56">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D57">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D58">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D59">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D60">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D61">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D62">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>65</v>
+        <v>208</v>
       </c>
       <c r="D63">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D64">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65">
         <v>314</v>
       </c>
@@ -2268,263 +2276,263 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="D66">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="D67">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
-        <v>69</v>
+        <v>211</v>
       </c>
       <c r="D68">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
       <c r="D69">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D70">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="D71">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D72">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="D73">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D74">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D75">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D76">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D77">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D78">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="D79">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D80">
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
-        <v>82</v>
+        <v>216</v>
       </c>
       <c r="D81">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D82">
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
       <c r="D83">
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D84">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D85">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D86">
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D87">
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D88">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="D89">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
-        <v>49</v>
+        <v>205</v>
       </c>
       <c r="D90">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D91">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D92">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
-        <v>93</v>
+        <v>219</v>
       </c>
       <c r="D93">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="D94">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D95">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="D96">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D97">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>19.466302949999999</v>
       </c>
@@ -2532,13 +2540,13 @@
         <v>-99.102743129999993</v>
       </c>
       <c r="C98" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="D98">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>19.392966090000002</v>
       </c>
@@ -2546,13 +2554,13 @@
         <v>-99.097602850000001</v>
       </c>
       <c r="C99" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="D99">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>19.431578720000001</v>
       </c>
@@ -2560,13 +2568,13 @@
         <v>-99.165748890000003</v>
       </c>
       <c r="C100" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="D100">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>19.395044899999998</v>
       </c>
@@ -2574,13 +2582,13 @@
         <v>-99.114076319999995</v>
       </c>
       <c r="C101" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D101">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>19.394239630000001</v>
       </c>
@@ -2588,13 +2596,13 @@
         <v>-99.1278054</v>
       </c>
       <c r="C102" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="D102">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>19.450036300000001</v>
       </c>
@@ -2602,13 +2610,13 @@
         <v>-99.146026829999997</v>
       </c>
       <c r="C103" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D103">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>19.389984070000001</v>
       </c>
@@ -2616,13 +2624,13 @@
         <v>-99.165484219999996</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D104">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>19.446602500000001</v>
       </c>
@@ -2630,13 +2638,13 @@
         <v>-99.149697739999993</v>
       </c>
       <c r="C105" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D105">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>19.498373059999999</v>
       </c>
@@ -2644,13 +2652,13 @@
         <v>-99.163132610000005</v>
       </c>
       <c r="C106" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D106">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>19.35924696</v>
       </c>
@@ -2658,13 +2666,13 @@
         <v>-99.176225360000004</v>
       </c>
       <c r="C107" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>19.430317809999998</v>
       </c>
@@ -2672,13 +2680,13 @@
         <v>-99.134924780000006</v>
       </c>
       <c r="C108" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D108">
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>19.447278990000001</v>
       </c>
@@ -2686,13 +2694,13 @@
         <v>-99.147939930000007</v>
       </c>
       <c r="C109" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D109">
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>19.498382929999998</v>
       </c>
@@ -2700,13 +2708,13 @@
         <v>-99.162936430000002</v>
       </c>
       <c r="C110" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="D110">
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>19.42145064</v>
       </c>
@@ -2714,13 +2722,13 @@
         <v>-99.159139039999999</v>
       </c>
       <c r="C111" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="D111">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>19.462903829999998</v>
       </c>
@@ -2728,517 +2736,517 @@
         <v>-99.141438480000005</v>
       </c>
       <c r="C112" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="D112">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C113" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="D113">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D114">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C115" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D115">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C116" t="s">
-        <v>116</v>
+        <v>220</v>
       </c>
       <c r="D116">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C117" t="s">
+        <v>66</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C118" t="s">
+        <v>67</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C119" t="s">
+        <v>90</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C120" t="s">
         <v>91</v>
       </c>
-      <c r="D117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C121" t="s">
+        <v>199</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C122" t="s">
         <v>92</v>
       </c>
-      <c r="D118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
-        <v>117</v>
-      </c>
-      <c r="D119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
-        <v>118</v>
-      </c>
-      <c r="D120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C121" t="s">
-        <v>33</v>
-      </c>
-      <c r="D121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C122" t="s">
-        <v>119</v>
-      </c>
       <c r="D122">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
       <c r="D123">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C124" t="s">
-        <v>121</v>
+        <v>222</v>
       </c>
       <c r="D124">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="D125">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C126" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="D126">
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="D127">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C128" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="D128">
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C129" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="D129">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="D130">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C131" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="D131">
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C132" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="D132">
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C133" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="D133">
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C134" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="D134">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C135" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D135">
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C136" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="D136">
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C137" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="D137">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C138" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="D138">
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C139" t="s">
-        <v>136</v>
+        <v>225</v>
       </c>
       <c r="D139">
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C140" t="s">
-        <v>137</v>
+        <v>226</v>
       </c>
       <c r="D140">
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C141" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="D141">
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C142" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="D142">
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C143" t="s">
-        <v>140</v>
+        <v>227</v>
       </c>
       <c r="D143">
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C144" t="s">
-        <v>141</v>
+        <v>228</v>
       </c>
       <c r="D144">
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C145" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="D145">
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="D146">
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C147" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="D147">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C148" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="D148">
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C149" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
       <c r="D149">
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C150" t="s">
-        <v>147</v>
+        <v>231</v>
       </c>
       <c r="D150">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C151" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="D151">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C152" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="D152">
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C153" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="D153">
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C154" t="s">
-        <v>151</v>
+        <v>233</v>
       </c>
       <c r="D154">
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C155" t="s">
-        <v>152</v>
+        <v>234</v>
       </c>
       <c r="D155">
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C156" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="D156">
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C157" t="s">
-        <v>116</v>
+        <v>220</v>
       </c>
       <c r="D157">
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C158" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="D158">
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C159" t="s">
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="D159">
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C160" t="s">
-        <v>156</v>
+        <v>236</v>
       </c>
       <c r="D160">
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C161" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="D161">
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C162" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="D162">
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C163" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="D163">
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C164" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="D164">
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C165" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="D165">
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C166" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D166">
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C167" t="s">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="D167">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C168" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="D168">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C169" t="s">
-        <v>164</v>
+        <v>240</v>
       </c>
       <c r="D169">
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C170" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="D170">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C171" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="D171">
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C172" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D172">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C173" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="D173">
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C174" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="D174">
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C175" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="D175">
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C176">
         <v>482</v>
       </c>
@@ -3246,591 +3254,591 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C177" t="s">
-        <v>164</v>
+        <v>240</v>
       </c>
       <c r="D177">
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C178" t="s">
-        <v>170</v>
+        <v>242</v>
       </c>
       <c r="D178">
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C179" t="s">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="D179">
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C180" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D180">
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C181" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D181">
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C182" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="D182">
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C183" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="D183">
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C184" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="D184">
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C185" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="D185">
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C186" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="D186">
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C187" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D187">
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C188" t="s">
-        <v>176</v>
+        <v>243</v>
       </c>
       <c r="D188">
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C189" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="D189">
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C190" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="D190">
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C191" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="D191">
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C192" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D192">
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C193" t="s">
-        <v>180</v>
+        <v>245</v>
       </c>
       <c r="D193">
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C194" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="D194">
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C195" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
       <c r="D195">
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C196" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="D196">
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C197" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="D197">
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C198" t="s">
-        <v>185</v>
+        <v>247</v>
       </c>
       <c r="D198">
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C199" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="D199">
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C200" t="s">
-        <v>187</v>
+        <v>248</v>
       </c>
       <c r="D200">
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C201" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
       <c r="D201">
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C202" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
       <c r="D202">
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C203" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="D203">
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C204" t="s">
-        <v>191</v>
+        <v>135</v>
       </c>
       <c r="D204">
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C205" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="D205">
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C206" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="D206">
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C207" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="D207">
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C208" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="D208">
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C209" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="D209">
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C210" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="D210">
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C211" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="D211">
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C212" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="D212">
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C213" t="s">
-        <v>199</v>
+        <v>251</v>
       </c>
       <c r="D213">
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C214" t="s">
-        <v>200</v>
+        <v>252</v>
       </c>
       <c r="D214">
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C215" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="D215">
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C216" t="s">
-        <v>202</v>
+        <v>253</v>
       </c>
       <c r="D216">
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C217" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="D217">
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C218" t="s">
-        <v>204</v>
+        <v>144</v>
       </c>
       <c r="D218">
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C219" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="D219">
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C220" t="s">
-        <v>206</v>
+        <v>146</v>
       </c>
       <c r="D220">
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C221" t="s">
-        <v>207</v>
+        <v>254</v>
       </c>
       <c r="D221">
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C222" t="s">
-        <v>208</v>
+        <v>147</v>
       </c>
       <c r="D222">
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C223" t="s">
-        <v>209</v>
+        <v>148</v>
       </c>
       <c r="D223">
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C224" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
       <c r="D224">
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C225" t="s">
-        <v>211</v>
+        <v>255</v>
       </c>
       <c r="D225">
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C226" t="s">
-        <v>51</v>
+        <v>206</v>
       </c>
       <c r="D226">
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C227" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
       <c r="D227">
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C228" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="D228">
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C229" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D229">
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C230" t="s">
-        <v>214</v>
+        <v>257</v>
       </c>
       <c r="D230">
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C231" t="s">
-        <v>215</v>
+        <v>151</v>
       </c>
       <c r="D231">
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C232" t="s">
-        <v>216</v>
+        <v>152</v>
       </c>
       <c r="D232">
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C233" t="s">
-        <v>217</v>
+        <v>153</v>
       </c>
       <c r="D233">
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C234" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="D234">
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C235" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="D235">
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C236" t="s">
-        <v>63</v>
+        <v>258</v>
       </c>
       <c r="D236">
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C237" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="D237">
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C238" t="s">
-        <v>221</v>
+        <v>156</v>
       </c>
       <c r="D238">
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C239" t="s">
-        <v>222</v>
+        <v>157</v>
       </c>
       <c r="D239">
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C240" t="s">
-        <v>223</v>
+        <v>158</v>
       </c>
       <c r="D240">
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C241" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="D241">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C242" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="D242">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C243" t="s">
-        <v>225</v>
+        <v>160</v>
       </c>
       <c r="D243">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C244" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="D244">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C245" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="D245">
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C246" t="s">
-        <v>228</v>
+        <v>162</v>
       </c>
       <c r="D246">
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C247" t="s">
-        <v>229</v>
+        <v>163</v>
       </c>
       <c r="D247">
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C248" t="s">
-        <v>230</v>
+        <v>164</v>
       </c>
       <c r="D248">
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C249" t="s">
-        <v>231</v>
+        <v>165</v>
       </c>
       <c r="D249">
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C250">
         <v>414</v>
       </c>
@@ -3838,159 +3846,159 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C251" t="s">
-        <v>232</v>
+        <v>166</v>
       </c>
       <c r="D251">
         <v>6</v>
       </c>
     </row>
-    <row r="252" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C252" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="D252">
         <v>6</v>
       </c>
     </row>
-    <row r="253" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C253" t="s">
-        <v>234</v>
+        <v>167</v>
       </c>
       <c r="D253">
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C254" t="s">
-        <v>235</v>
+        <v>168</v>
       </c>
       <c r="D254">
         <v>6</v>
       </c>
     </row>
-    <row r="255" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C255" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="D255">
         <v>6</v>
       </c>
     </row>
-    <row r="256" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C256" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="D256">
         <v>6</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C257" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D257">
         <v>6</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C258" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="D258">
         <v>6</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C259" t="s">
-        <v>238</v>
+        <v>170</v>
       </c>
       <c r="D259">
         <v>6</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C260" t="s">
-        <v>239</v>
+        <v>171</v>
       </c>
       <c r="D260">
         <v>6</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C261" t="s">
-        <v>240</v>
+        <v>172</v>
       </c>
       <c r="D261">
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C262" t="s">
-        <v>241</v>
+        <v>173</v>
       </c>
       <c r="D262">
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C263" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D263">
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C264" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="D264">
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C265" t="s">
-        <v>242</v>
+        <v>174</v>
       </c>
       <c r="D265">
         <v>7</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C266" t="s">
-        <v>243</v>
+        <v>175</v>
       </c>
       <c r="D266">
         <v>7</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C267" t="s">
-        <v>244</v>
+        <v>176</v>
       </c>
       <c r="D267">
         <v>7</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C268" t="s">
-        <v>245</v>
+        <v>177</v>
       </c>
       <c r="D268">
         <v>7</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C269" t="s">
-        <v>246</v>
+        <v>178</v>
       </c>
       <c r="D269">
         <v>7</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>19.46309604</v>
       </c>
@@ -3998,13 +4006,13 @@
         <v>-99.152662770000006</v>
       </c>
       <c r="C270" t="s">
-        <v>247</v>
+        <v>179</v>
       </c>
       <c r="D270">
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>19.462690120000001</v>
       </c>
@@ -4012,13 +4020,13 @@
         <v>-99.141743169999998</v>
       </c>
       <c r="C271" t="s">
-        <v>248</v>
+        <v>180</v>
       </c>
       <c r="D271">
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>19.39346222</v>
       </c>
@@ -4026,13 +4034,13 @@
         <v>-99.113111959999998</v>
       </c>
       <c r="C272" t="s">
-        <v>249</v>
+        <v>181</v>
       </c>
       <c r="D272">
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>19.437390400000002</v>
       </c>
@@ -4040,13 +4048,13 @@
         <v>-99.135057290000006</v>
       </c>
       <c r="C273" t="s">
-        <v>250</v>
+        <v>182</v>
       </c>
       <c r="D273">
         <v>4</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>19.388578469999999</v>
       </c>
@@ -4054,13 +4062,13 @@
         <v>-99.165692460000002</v>
       </c>
       <c r="C274" t="s">
-        <v>251</v>
+        <v>183</v>
       </c>
       <c r="D274">
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>19.394297949999999</v>
       </c>
@@ -4068,13 +4076,13 @@
         <v>-99.126046930000001</v>
       </c>
       <c r="C275" t="s">
-        <v>252</v>
+        <v>184</v>
       </c>
       <c r="D275">
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>19.394854509999998</v>
       </c>
@@ -4082,13 +4090,13 @@
         <v>-99.117402040000002</v>
       </c>
       <c r="C276" t="s">
-        <v>253</v>
+        <v>185</v>
       </c>
       <c r="D276">
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>19.360329159999999</v>
       </c>
@@ -4096,13 +4104,13 @@
         <v>-99.176312280000005</v>
       </c>
       <c r="C277" t="s">
-        <v>254</v>
+        <v>186</v>
       </c>
       <c r="D277">
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>19.487242380000001</v>
       </c>
@@ -4110,13 +4118,13 @@
         <v>-99.127975820000003</v>
       </c>
       <c r="C278" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
       <c r="D278">
         <v>6</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>19.4770751</v>
       </c>
@@ -4124,13 +4132,13 @@
         <v>-99.152223359999994</v>
       </c>
       <c r="C279" t="s">
-        <v>256</v>
+        <v>188</v>
       </c>
       <c r="D279">
         <v>3</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>19.497487360000001</v>
       </c>
@@ -4138,13 +4146,13 @@
         <v>-99.155208860000002</v>
       </c>
       <c r="C280" t="s">
-        <v>257</v>
+        <v>189</v>
       </c>
       <c r="D280">
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>19.47869158</v>
       </c>
@@ -4152,13 +4160,13 @@
         <v>-99.094633790000003</v>
       </c>
       <c r="C281" t="s">
-        <v>258</v>
+        <v>190</v>
       </c>
       <c r="D281">
         <v>6</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>19.431281129999999</v>
       </c>
@@ -4166,13 +4174,13 @@
         <v>-99.164984290000007</v>
       </c>
       <c r="C282" t="s">
-        <v>259</v>
+        <v>191</v>
       </c>
       <c r="D282">
         <v>7</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>19.45804489</v>
       </c>
@@ -4180,13 +4188,13 @@
         <v>-99.134057990000002</v>
       </c>
       <c r="C283" t="s">
-        <v>260</v>
+        <v>192</v>
       </c>
       <c r="D283">
         <v>7</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>19.47652076</v>
       </c>
@@ -4194,7 +4202,7 @@
         <v>-99.152118110000004</v>
       </c>
       <c r="C284" t="s">
-        <v>261</v>
+        <v>193</v>
       </c>
       <c r="D284">
         <v>3</v>

</xml_diff>